<commit_message>
Welcome modified for clients
</commit_message>
<xml_diff>
--- a/Tables pages concepts.xlsx
+++ b/Tables pages concepts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laravel\psychologyTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4F2D1C-A733-45BF-92A2-C9A3F5CB7738}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1215018-3ADE-4537-A655-FA74588640C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22118" windowHeight="8536" xr2:uid="{CE7EEF5A-B53F-4026-870A-F3CB51798D78}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>tables</t>
   </si>
@@ -60,9 +60,6 @@
     <t>qty to fake</t>
   </si>
   <si>
-    <t>users (psychologist)</t>
-  </si>
-  <si>
     <t>clients</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>client will be able to log in with the given credentials. There is no registering for clients.</t>
   </si>
   <si>
-    <t>psychologist(True/False)</t>
-  </si>
-  <si>
     <t>test_name</t>
   </si>
   <si>
@@ -102,10 +96,22 @@
     <t>answer_value</t>
   </si>
   <si>
-    <t>negative_item(true/false)</t>
-  </si>
-  <si>
     <t>Only one dimensional tests are planned, with Likert scales.</t>
+  </si>
+  <si>
+    <t>client(True/False)</t>
+  </si>
+  <si>
+    <t>psychologist_id</t>
+  </si>
+  <si>
+    <t>Is the app generally ment for online use, or it is ment to be used during a live therapy? DURING LIVE THERAPY</t>
+  </si>
+  <si>
+    <t>Is one app for one psychologist, or one app for many psychologist? ONE APP FOR MANY PSYCHOLOGIST</t>
+  </si>
+  <si>
+    <t>Should clients log in by themselves, or should they be added by the psycholgist? THEY SHOULD BE ADDED BY THE PSYCHOLOGIST, DURING A LIVE SESSION</t>
   </si>
 </sst>
 </file>
@@ -532,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562C513A-CEF2-47DE-9D7A-6847428F89B6}">
-  <dimension ref="B2:M22"/>
+  <dimension ref="B2:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,7 +550,7 @@
     <col min="2" max="2" width="2.59765625" style="11" customWidth="1"/>
     <col min="3" max="3" width="15.69921875" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="10.19921875" customWidth="1"/>
+    <col min="5" max="5" width="12.796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.3984375" customWidth="1"/>
     <col min="7" max="7" width="21.09765625" customWidth="1"/>
     <col min="8" max="8" width="13.296875" bestFit="1" customWidth="1"/>
@@ -588,12 +594,12 @@
         <v>6</v>
       </c>
       <c r="M3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C4" s="17" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>3</v>
@@ -610,18 +616,18 @@
         <v>4</v>
       </c>
       <c r="M4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C5" s="17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="17"/>
@@ -632,61 +638,43 @@
         <v>3</v>
       </c>
       <c r="M5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C6" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="17"/>
       <c r="J6" s="8"/>
       <c r="M6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C7" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>15</v>
-      </c>
       <c r="F7" s="8"/>
       <c r="G7" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="17"/>
       <c r="J7" s="8"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C8" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>14</v>
-      </c>
       <c r="F8" s="8"/>
       <c r="G8" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="17"/>
@@ -698,7 +686,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="8"/>
       <c r="G9" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="17"/>
@@ -754,9 +742,11 @@
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="16"/>
@@ -768,10 +758,10 @@
         <v>2</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>5</v>
@@ -785,13 +775,13 @@
         <v>3</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -802,21 +792,21 @@
         <v>4</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="F20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H20" s="16"/>
+        <v>5</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="18"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="14">
@@ -839,6 +829,21 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="16"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A6:A15">

</xml_diff>